<commit_message>
add cpu performance to sheets
</commit_message>
<xml_diff>
--- a/LOG8430E_redis_results.xlsx
+++ b/LOG8430E_redis_results.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thierry/Desktop/LOG8430E_TP3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450985DF-5A72-5548-A406-BAAB7EE30009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B71A8A-9E05-EC48-8D73-0B2199D9F4EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tps-25" sheetId="1" r:id="rId1"/>
     <sheet name="tps-500" sheetId="2" r:id="rId2"/>
     <sheet name="tps-1000" sheetId="3" r:id="rId3"/>
     <sheet name="results" sheetId="4" r:id="rId4"/>
+    <sheet name="cpuperformance" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1677" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2101" uniqueCount="144">
   <si>
     <t>##################################################################################</t>
   </si>
@@ -211,17 +212,282 @@
   </si>
   <si>
     <t>Average Throughput (ops/sec)</t>
+  </si>
+  <si>
+    <t>0B / 0B</t>
+  </si>
+  <si>
+    <t>secondary2</t>
+  </si>
+  <si>
+    <t>05171fe267b1</t>
+  </si>
+  <si>
+    <t>secondary3</t>
+  </si>
+  <si>
+    <t>f9a1f9c4c25c</t>
+  </si>
+  <si>
+    <t>primary</t>
+  </si>
+  <si>
+    <t>d7006a18086b</t>
+  </si>
+  <si>
+    <t>secondary1</t>
+  </si>
+  <si>
+    <t>62b9b8e9d2ef</t>
+  </si>
+  <si>
+    <t>16MB</t>
+  </si>
+  <si>
+    <t>193kB /</t>
+  </si>
+  <si>
+    <t>15.8MB / 44.8MB</t>
+  </si>
+  <si>
+    <t>6.121MiB / 15.55GiB</t>
+  </si>
+  <si>
+    <t>redis_redis-master_1</t>
+  </si>
+  <si>
+    <t>83aca997f9e0</t>
+  </si>
+  <si>
+    <t>16.2MB</t>
+  </si>
+  <si>
+    <t>12.7MB / 515kB</t>
+  </si>
+  <si>
+    <t>6.363MiB / 15.55GiB</t>
+  </si>
+  <si>
+    <t>redis_redis-replica_2</t>
+  </si>
+  <si>
+    <t>a0cabf92bf36</t>
+  </si>
+  <si>
+    <t>12.7MB / 505kB</t>
+  </si>
+  <si>
+    <t>6.355MiB / 15.55GiB</t>
+  </si>
+  <si>
+    <t>redis_redis-replica_1</t>
+  </si>
+  <si>
+    <t>91da5ba107bd</t>
+  </si>
+  <si>
+    <t>12.7MB / 529kB</t>
+  </si>
+  <si>
+    <t>6.359MiB / 15.55GiB</t>
+  </si>
+  <si>
+    <t>redis_redis-replica_3</t>
+  </si>
+  <si>
+    <t>a764c0ca7263</t>
+  </si>
+  <si>
+    <t>PIDS</t>
+  </si>
+  <si>
+    <t>/O</t>
+  </si>
+  <si>
+    <t>BLOCK I</t>
+  </si>
+  <si>
+    <t>NET I/O</t>
+  </si>
+  <si>
+    <t>MEM %</t>
+  </si>
+  <si>
+    <t>MEM USAGE / LIMIT</t>
+  </si>
+  <si>
+    <t>CPU %</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>CONTAINER ID</t>
+  </si>
+  <si>
+    <t>15MB</t>
+  </si>
+  <si>
+    <t>6.148MiB / 15.55GiB</t>
+  </si>
+  <si>
+    <t>15.2MB</t>
+  </si>
+  <si>
+    <t>6.391MiB / 15.55GiB</t>
+  </si>
+  <si>
+    <t>15.3MB</t>
+  </si>
+  <si>
+    <t>12.7MB / 504kB</t>
+  </si>
+  <si>
+    <t>6.383MiB / 15.55GiB</t>
+  </si>
+  <si>
+    <t>184kB /</t>
+  </si>
+  <si>
+    <t>11.5MB / 498kB</t>
+  </si>
+  <si>
+    <t>14.7MB</t>
+  </si>
+  <si>
+    <t>180kB /</t>
+  </si>
+  <si>
+    <t>14.2MB / 40.7MB</t>
+  </si>
+  <si>
+    <t>11.3MB / 479kB</t>
+  </si>
+  <si>
+    <t>6.055MiB / 15.55GiB</t>
+  </si>
+  <si>
+    <t>11.3MB / 469kB</t>
+  </si>
+  <si>
+    <t>6.035MiB / 15.55GiB</t>
+  </si>
+  <si>
+    <t>11.3MB / 492kB</t>
+  </si>
+  <si>
+    <t>6.062MiB / 15.55GiB</t>
+  </si>
+  <si>
+    <t>11.3MB / 468kB</t>
+  </si>
+  <si>
+    <t>14.6MB</t>
+  </si>
+  <si>
+    <t>14.1MB / 39.4MB</t>
+  </si>
+  <si>
+    <t>6.125MiB / 15.55GiB</t>
+  </si>
+  <si>
+    <t>11.3MB / 478kB</t>
+  </si>
+  <si>
+    <t>6.492MiB / 15.55GiB</t>
+  </si>
+  <si>
+    <t>6.48MiB / 15.55GiB</t>
+  </si>
+  <si>
+    <t>11.3MB / 491kB</t>
+  </si>
+  <si>
+    <t>6.414MiB / 15.55GiB</t>
+  </si>
+  <si>
+    <t>13.5MB</t>
+  </si>
+  <si>
+    <t>168kB /</t>
+  </si>
+  <si>
+    <t>12.6MB / 35.3MB</t>
+  </si>
+  <si>
+    <t>5.922MiB / 15.55GiB</t>
+  </si>
+  <si>
+    <t>13.7MB</t>
+  </si>
+  <si>
+    <t>10MB / 445kB</t>
+  </si>
+  <si>
+    <t>6.109MiB / 15.55GiB</t>
+  </si>
+  <si>
+    <t>10MB / 434kB</t>
+  </si>
+  <si>
+    <t>6.082MiB / 15.55GiB</t>
+  </si>
+  <si>
+    <t>10MB / 457kB</t>
+  </si>
+  <si>
+    <t>6.18MiB / 15.55GiB</t>
+  </si>
+  <si>
+    <t>10MB / 433kB</t>
+  </si>
+  <si>
+    <t>13.3MB</t>
+  </si>
+  <si>
+    <t>156kB /</t>
+  </si>
+  <si>
+    <t>12.2MB / 34.5MB</t>
+  </si>
+  <si>
+    <t>5.883MiB / 15.55GiB</t>
+  </si>
+  <si>
+    <t>9.82MB / 415kB</t>
+  </si>
+  <si>
+    <t>6.43MiB / 15.55GiB</t>
+  </si>
+  <si>
+    <t>9.82MB / 403kB</t>
+  </si>
+  <si>
+    <t>6.434MiB / 15.55GiB</t>
+  </si>
+  <si>
+    <t>9.82MB / 426kB</t>
+  </si>
+  <si>
+    <t>6.348MiB / 15.55GiB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -380,40 +646,41 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -423,9 +690,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{971BCF6A-2436-824B-9B86-7D5280B2B884}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -10127,7 +10397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80A30658-965C-484C-9C04-9200B800EB27}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -10135,4 +10405,2014 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B8D10F-DE65-A345-A543-886720C7F693}">
+  <dimension ref="A1:I72"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="29"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="30">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="E2" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="I2" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="30">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="E3" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F3" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="H3" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="I3" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="30">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="E4" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="H4" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="I4" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="30">
+        <v>1.5E-3</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="H5" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="I5" s="29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="30">
+        <v>0</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="30">
+        <v>0</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I6" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="30">
+        <v>0</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="30">
+        <v>0</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="30">
+        <v>0</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="30">
+        <v>0</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="30">
+        <v>0</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="30">
+        <v>0</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="G10" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="H10" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="I10" s="29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="30">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="E11" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F11" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="G11" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="H11" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="I11" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="30">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="E12" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="G12" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="H12" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="I12" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="30">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="E13" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="G13" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="H13" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="I13" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="30">
+        <v>1.5E-3</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="E14" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="G14" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="H14" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="I14" s="29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="30">
+        <v>0</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="30">
+        <v>0</v>
+      </c>
+      <c r="F15" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I15" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="30">
+        <v>0</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="30">
+        <v>0</v>
+      </c>
+      <c r="F16" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I16" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="30">
+        <v>0</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="30">
+        <v>0</v>
+      </c>
+      <c r="F17" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I17" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="30">
+        <v>0</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="30">
+        <v>0</v>
+      </c>
+      <c r="F18" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I18" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="G19" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="H19" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="I19" s="29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="30">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="E20" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F20" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="G20" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="H20" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="I20" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" s="30">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="E21" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F21" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="G21" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="H21" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="I21" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="30">
+        <v>1.5E-3</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="E22" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F22" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="G22" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="H22" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="I22" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="30">
+        <v>1.5E-3</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="E23" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F23" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="G23" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="H23" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="I23" s="29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="30">
+        <v>0</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" s="30">
+        <v>0</v>
+      </c>
+      <c r="F24" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G24" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I24" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="30">
+        <v>0</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" s="30">
+        <v>0</v>
+      </c>
+      <c r="F25" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G25" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I25" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="30">
+        <v>0</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="30">
+        <v>0</v>
+      </c>
+      <c r="F26" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G26" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I26" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="30">
+        <v>0</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="30">
+        <v>0</v>
+      </c>
+      <c r="F27" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G27" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I27" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="E28" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="F28" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="G28" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="H28" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="I28" s="29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" s="30">
+        <v>1.9E-3</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="E29" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F29" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="G29" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="H29" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="I29" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="30">
+        <v>1.9E-3</v>
+      </c>
+      <c r="D30" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="E30" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F30" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="G30" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="H30" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="I30" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="30">
+        <v>2E-3</v>
+      </c>
+      <c r="D31" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="E31" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F31" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="G31" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="H31" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="I31" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="30">
+        <v>2.5700000000000001E-2</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="E32" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F32" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="G32" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="H32" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="I32" s="29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="30">
+        <v>0</v>
+      </c>
+      <c r="D33" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33" s="30">
+        <v>0</v>
+      </c>
+      <c r="F33" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G33" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I33" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" s="30">
+        <v>0</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E34" s="30">
+        <v>0</v>
+      </c>
+      <c r="F34" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G34" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I34" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="30">
+        <v>0</v>
+      </c>
+      <c r="D35" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E35" s="30">
+        <v>0</v>
+      </c>
+      <c r="F35" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G35" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I35" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="30">
+        <v>0</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E36" s="30">
+        <v>0</v>
+      </c>
+      <c r="F36" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G36" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I36" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B37" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D37" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="F37" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="G37" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="H37" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="I37" s="29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" s="30">
+        <v>2.0999999999999999E-3</v>
+      </c>
+      <c r="D38" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="E38" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F38" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="G38" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="H38" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="I38" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="30">
+        <v>2.0999999999999999E-3</v>
+      </c>
+      <c r="D39" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="E39" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F39" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="G39" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="H39" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="I39" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" s="30">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="D40" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="E40" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F40" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="G40" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="H40" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="I40" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C41" s="30">
+        <v>7.7100000000000002E-2</v>
+      </c>
+      <c r="D41" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="E41" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F41" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="G41" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="H41" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="I41" s="29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B42" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="30">
+        <v>0</v>
+      </c>
+      <c r="D42" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E42" s="30">
+        <v>0</v>
+      </c>
+      <c r="F42" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G42" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I42" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C43" s="30">
+        <v>0</v>
+      </c>
+      <c r="D43" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E43" s="30">
+        <v>0</v>
+      </c>
+      <c r="F43" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G43" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I43" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B44" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C44" s="30">
+        <v>0</v>
+      </c>
+      <c r="D44" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E44" s="30">
+        <v>0</v>
+      </c>
+      <c r="F44" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G44" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I44" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B45" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C45" s="30">
+        <v>0</v>
+      </c>
+      <c r="D45" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E45" s="30">
+        <v>0</v>
+      </c>
+      <c r="F45" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G45" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I45" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B46" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C46" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D46" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="E46" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="F46" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="G46" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="H46" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="I46" s="29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B47" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C47" s="30">
+        <v>1.5E-3</v>
+      </c>
+      <c r="D47" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="E47" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F47" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="G47" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="H47" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="I47" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B48" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C48" s="30">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="D48" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="E48" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F48" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="G48" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="H48" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="I48" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B49" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C49" s="30">
+        <v>1.8E-3</v>
+      </c>
+      <c r="D49" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="E49" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F49" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="G49" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="H49" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="I49" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B50" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C50" s="30">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="D50" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="E50" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F50" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="G50" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="H50" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="I50" s="29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B51" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C51" s="30">
+        <v>0</v>
+      </c>
+      <c r="D51" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E51" s="30">
+        <v>0</v>
+      </c>
+      <c r="F51" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G51" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I51" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B52" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52" s="30">
+        <v>0</v>
+      </c>
+      <c r="D52" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E52" s="30">
+        <v>0</v>
+      </c>
+      <c r="F52" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G52" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I52" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B53" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C53" s="30">
+        <v>0</v>
+      </c>
+      <c r="D53" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E53" s="30">
+        <v>0</v>
+      </c>
+      <c r="F53" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G53" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I53" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B54" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C54" s="30">
+        <v>0</v>
+      </c>
+      <c r="D54" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E54" s="30">
+        <v>0</v>
+      </c>
+      <c r="F54" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G54" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I54" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B55" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C55" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D55" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="E55" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="F55" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="G55" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="H55" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="I55" s="29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B56" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C56" s="30">
+        <v>6.6E-3</v>
+      </c>
+      <c r="D56" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E56" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F56" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="G56" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="H56" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="I56" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B57" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C57" s="30">
+        <v>6.3200000000000006E-2</v>
+      </c>
+      <c r="D57" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="E57" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F57" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="G57" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="H57" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="I57" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B58" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C58" s="30">
+        <v>6.0400000000000002E-2</v>
+      </c>
+      <c r="D58" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="E58" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F58" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="G58" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="H58" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="I58" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B59" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C59" s="30">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="D59" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="E59" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F59" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="G59" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="H59" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="I59" s="29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B60" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C60" s="30">
+        <v>0</v>
+      </c>
+      <c r="D60" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E60" s="30">
+        <v>0</v>
+      </c>
+      <c r="F60" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G60" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I60" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B61" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C61" s="30">
+        <v>0</v>
+      </c>
+      <c r="D61" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E61" s="30">
+        <v>0</v>
+      </c>
+      <c r="F61" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G61" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I61" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B62" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C62" s="30">
+        <v>0</v>
+      </c>
+      <c r="D62" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E62" s="30">
+        <v>0</v>
+      </c>
+      <c r="F62" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G62" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I62" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B63" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C63" s="30">
+        <v>0</v>
+      </c>
+      <c r="D63" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E63" s="30">
+        <v>0</v>
+      </c>
+      <c r="F63" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G63" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I63" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B64" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C64" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D64" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="E64" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="F64" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="G64" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="H64" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="I64" s="29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B65" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C65" s="30">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="D65" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E65" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F65" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="G65" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="H65" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="I65" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B66" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C66" s="30">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="D66" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="E66" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F66" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="G66" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="H66" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="I66" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B67" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C67" s="30">
+        <v>1.5E-3</v>
+      </c>
+      <c r="D67" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="E67" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F67" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="G67" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="H67" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="I67" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B68" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C68" s="30">
+        <v>1.5E-3</v>
+      </c>
+      <c r="D68" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="E68" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F68" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="G68" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="H68" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="I68" s="29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B69" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C69" s="30">
+        <v>0</v>
+      </c>
+      <c r="D69" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E69" s="30">
+        <v>0</v>
+      </c>
+      <c r="F69" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G69" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I69" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B70" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C70" s="30">
+        <v>0</v>
+      </c>
+      <c r="D70" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E70" s="30">
+        <v>0</v>
+      </c>
+      <c r="F70" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G70" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I70" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A71" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B71" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C71" s="30">
+        <v>0</v>
+      </c>
+      <c r="D71" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E71" s="30">
+        <v>0</v>
+      </c>
+      <c r="F71" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G71" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I71" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A72" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B72" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C72" s="30">
+        <v>0</v>
+      </c>
+      <c r="D72" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E72" s="30">
+        <v>0</v>
+      </c>
+      <c r="F72" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G72" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I72" s="29">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
a bit of formating
</commit_message>
<xml_diff>
--- a/LOG8430E_redis_results.xlsx
+++ b/LOG8430E_redis_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thierry/Desktop/LOG8430E_TP3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34013D9A-8264-6242-9EF6-3B3ACBC35134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF34676-4752-9B47-9229-ACFC82C4D1EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1078,7 +1078,7 @@
   <dimension ref="A1:N285"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4245,9 +4245,12 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="9" max="9" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" ht="28" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -7399,7 +7402,7 @@
   <dimension ref="A1:O285"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:N19"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10562,7 +10565,7 @@
   <dimension ref="A1:S72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O33" sqref="O33"/>
+      <selection activeCell="S36" sqref="S36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
created a diagram for 25 tps
</commit_message>
<xml_diff>
--- a/LOG8430E_redis_results.xlsx
+++ b/LOG8430E_redis_results.xlsx
@@ -8,17 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thierry/Desktop/LOG8430E_TP3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF34676-4752-9B47-9229-ACFC82C4D1EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C44CC78-C285-9940-A4B5-E9083E39129D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tps-25" sheetId="1" r:id="rId1"/>
     <sheet name="tps-500" sheetId="2" r:id="rId2"/>
     <sheet name="tps-1000" sheetId="3" r:id="rId3"/>
     <sheet name="cpu-mem-1000" sheetId="6" r:id="rId4"/>
-    <sheet name="results" sheetId="4" r:id="rId5"/>
+    <sheet name="results" sheetId="7" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'tps-25'!$K$24</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'tps-25'!$L$15:$L$17</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'tps-25'!$M$15:$M$17</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'tps-25'!$M$16:$M$17</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'tps-25'!$K$24</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'tps-25'!$K$24</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'tps-25'!$L$15:$L$17</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'tps-25'!$M$15:$M$17</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'tps-25'!$M$16:$M$17</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -755,7 +766,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -856,6 +867,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -872,6 +886,1052 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Average</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> Latencies of Redis Obtained With YCSB With a Throughput of 25 (ops/s)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'tps-25'!$L$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>READ</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'tps-25'!$K$15:$K$17</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Workload 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Workload 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Workload 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'tps-25'!$L$15:$L$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>515.10566666666671</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>666.00411489645933</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>670.74682096041306</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2E88-A34E-8E0A-96986A3DC8D9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'tps-25'!$M$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WRITES</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'tps-25'!$K$15:$K$17</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Workload 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Workload 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Workload 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'tps-25'!$M$15:$M$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="1">
+                  <c:v>1040.9225054652568</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>796.91455621109969</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2E88-A34E-8E0A-96986A3DC8D9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="487141040"/>
+        <c:axId val="487142768"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="487141040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="487142768"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="487142768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Average</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> Latency (us)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="487141040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1155700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69F2605E-E4AB-F59C-775E-B85E85FA381F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1075,10 +2135,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N285"/>
+  <dimension ref="A1:S285"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="Q35" sqref="Q35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1088,8 +2148,8 @@
     <col min="12" max="14" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:14" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:19" ht="28" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1108,7 +2168,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1127,7 +2187,7 @@
       </c>
       <c r="N3" s="7"/>
     </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1156,7 +2216,7 @@
         <v>24.933303413369199</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1182,7 +2242,7 @@
         <v>24.983760555638799</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1208,7 +2268,7 @@
         <v>24.980015987210201</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1231,7 +2291,7 @@
         <v>24.9868818870093</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1257,7 +2317,7 @@
         <v>24.975024975024901</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -1283,7 +2343,7 @@
         <v>24.977520231791299</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1306,7 +2366,7 @@
         <v>24.968165588874101</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -1332,7 +2392,7 @@
         <v>24.967542195146301</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -1358,7 +2418,7 @@
         <v>24.968789013732799</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -1372,7 +2432,7 @@
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -1390,7 +2450,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
@@ -1408,8 +2468,13 @@
         <v>515.10566666666671</v>
       </c>
       <c r="M15" s="10"/>
-    </row>
-    <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O15" s="12"/>
+      <c r="P15" s="54"/>
+      <c r="Q15" s="54"/>
+      <c r="R15" s="54"/>
+      <c r="S15" s="53"/>
+    </row>
+    <row r="16" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
@@ -1430,8 +2495,13 @@
         <f>AVERAGE(M5,M8,M11)</f>
         <v>1040.9225054652568</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="O16" s="6"/>
+      <c r="P16" s="54"/>
+      <c r="Q16" s="52"/>
+      <c r="R16" s="52"/>
+      <c r="S16" s="53"/>
+    </row>
+    <row r="17" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
@@ -1452,8 +2522,13 @@
         <f>AVERAGE(M6,M9,M12)</f>
         <v>796.91455621109969</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="O17" s="6"/>
+      <c r="P17" s="52"/>
+      <c r="Q17" s="52"/>
+      <c r="R17" s="52"/>
+      <c r="S17" s="53"/>
+    </row>
+    <row r="18" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -1464,7 +2539,7 @@
         <v>11655</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
@@ -1482,7 +2557,7 @@
         <v>24.971222649755209</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
@@ -1493,7 +2568,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
         <v>17</v>
       </c>
@@ -1504,7 +2579,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -1515,7 +2590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -1526,7 +2601,7 @@
         <v>1340</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -1537,7 +2612,7 @@
         <v>1340</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -1548,7 +2623,7 @@
         <v>1340</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -1559,7 +2634,7 @@
         <v>1340</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1570,17 +2645,17 @@
         <v>1340</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
@@ -1591,7 +2666,7 @@
         <v>40026</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>2</v>
       </c>
@@ -4230,6 +5305,7 @@
     <mergeCell ref="L2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4240,8 +5316,8 @@
   </sheetPr>
   <dimension ref="A1:N285"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10564,8 +11640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B8D10F-DE65-A345-A543-886720C7F693}">
   <dimension ref="A1:S72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S36" sqref="S36"/>
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M51" sqref="M51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13389,11 +14465,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80A30658-965C-484C-9C04-9200B800EB27}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FBFCAC3-55BC-944C-B7B3-C5C9963935EC}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
add hyperledger fabric data
</commit_message>
<xml_diff>
--- a/LOG8430E_redis_results.xlsx
+++ b/LOG8430E_redis_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thierry/Desktop/LOG8430E_TP3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4FD5A9-B7A4-174E-8321-93A824F7E098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E24C64-E10E-054B-8394-C4044E398942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1480" yWindow="500" windowWidth="36920" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tps-25" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,14 @@
     <sheet name="cpu-mem-1000" sheetId="6" r:id="rId4"/>
     <sheet name="results" sheetId="7" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">results!$C$20</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">results!$C$21:$C$23</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">results!$D$20</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">results!$D$21:$D$23</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">results!$E$20</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">results!$F$21:$F$23</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
   <extLst>
@@ -38,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2174" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2191" uniqueCount="174">
   <si>
     <t>##################################################################################</t>
   </si>
@@ -515,6 +523,57 @@
     <t>Average
 throughput</t>
   </si>
+  <si>
+    <t>Hyperledger</t>
+  </si>
+  <si>
+    <t>Mesure</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Latency (s) read</t>
+  </si>
+  <si>
+    <t>Latency (s) write</t>
+  </si>
+  <si>
+    <t>Send Rate (TPS) read</t>
+  </si>
+  <si>
+    <t>Send Rate (TPS) write</t>
+  </si>
+  <si>
+    <t>CPU read</t>
+  </si>
+  <si>
+    <t>CPU write</t>
+  </si>
+  <si>
+    <t>Memory (avg) MB read</t>
+  </si>
+  <si>
+    <t>Memory (avg) MB write</t>
+  </si>
+  <si>
+    <t>Traffic In MB read</t>
+  </si>
+  <si>
+    <t>Traffic In MB write</t>
+  </si>
+  <si>
+    <t>Traffic Out MB write</t>
+  </si>
+  <si>
+    <t>Traffic Out MB read</t>
+  </si>
 </sst>
 </file>
 
@@ -800,7 +859,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -943,6 +1002,16 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1072,6 +1141,60 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'tps-25'!$K$15:$K$17</c:f>
@@ -1137,6 +1260,60 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'tps-25'!$K$15:$K$17</c:f>
@@ -1580,18 +1757,18 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>results!$F$21:$F$23</c:f>
+              <c:f>results!$E$21:$E$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>24.971222649755209</c:v>
+                  <c:v>670.74682096041306</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>494.64248697497646</c:v>
+                  <c:v>461.67304458513331</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>972.59089191969053</c:v>
+                  <c:v>339.96199677938768</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1927,7 +2104,8 @@
         <c:axId val="488151856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1000"/>
+          <c:max val="700"/>
+          <c:min val="200"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2136,6 +2314,609 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Impact of Throughput on WRITE Latencies</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>results!$J$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>workload 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>results!$K$21:$K$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>24.971222649755209</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>494.64248697497646</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>972.59089191969053</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>results!$J$21:$J$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>796.91455621109969</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>566.46727886794577</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>387.72318745864965</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B775-A041-B29E-BDBF7BE475C4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>results!$I$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>workload 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:forward val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>results!$K$21:$K$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>24.971222649755209</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>494.64248697497646</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>972.59089191969053</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>results!$I$21:$I$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1040.9225054652568</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>530.72116225604634</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>290.50553667361635</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B775-A041-B29E-BDBF7BE475C4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="390580368"/>
+        <c:axId val="390582640"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="390580368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Average</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> Throughput (ops/s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="390582640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="390582640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="200"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Latency</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> (us)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="390580368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2177,6 +2958,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3235,14 +4056,530 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1155700</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:colOff>1016000</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
@@ -3286,10 +4623,10 @@
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3309,6 +4646,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C465ACFB-4492-7A40-0C10-558926C88261}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3518,10 +4891,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:R285"/>
+  <dimension ref="A1:S285"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14:M19"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3529,10 +4902,11 @@
     <col min="9" max="9" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.33203125" customWidth="1"/>
     <col min="12" max="14" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:18" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:19" ht="28" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3550,8 +4924,14 @@
       <c r="N2" s="19" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P2" s="5"/>
+      <c r="Q2" s="69" t="s">
+        <v>157</v>
+      </c>
+      <c r="R2" s="69"/>
+      <c r="S2" s="70"/>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -3569,8 +4949,20 @@
         <v>43</v>
       </c>
       <c r="N3" s="7"/>
-    </row>
-    <row r="4" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="P3" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q3" s="68" t="s">
+        <v>159</v>
+      </c>
+      <c r="R3" s="68" t="s">
+        <v>160</v>
+      </c>
+      <c r="S3" s="71" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -3597,8 +4989,20 @@
         <f>C5</f>
         <v>24.933303413369199</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P4" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q4" s="72">
+        <v>0.02</v>
+      </c>
+      <c r="R4" s="72">
+        <v>0.01</v>
+      </c>
+      <c r="S4" s="10">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -3623,8 +5027,18 @@
         <f>C32</f>
         <v>24.983760555638799</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P5" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q5" s="72"/>
+      <c r="R5" s="72">
+        <v>0.48</v>
+      </c>
+      <c r="S5" s="10">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -3649,8 +5063,20 @@
         <f>C66</f>
         <v>24.980015987210201</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P6" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q6" s="72">
+        <v>25.4</v>
+      </c>
+      <c r="R6" s="72">
+        <v>25.2</v>
+      </c>
+      <c r="S6" s="10">
+        <v>25.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -3671,8 +5097,18 @@
         <f>C100</f>
         <v>24.9868818870093</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P7" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q7" s="72"/>
+      <c r="R7" s="72">
+        <v>25.2</v>
+      </c>
+      <c r="S7" s="10">
+        <v>25.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -3697,8 +5133,14 @@
         <f>C127</f>
         <v>24.975024975024901</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P8" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q8" s="72"/>
+      <c r="R8" s="72"/>
+      <c r="S8" s="10"/>
+    </row>
+    <row r="9" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -3723,8 +5165,14 @@
         <f>C161</f>
         <v>24.977520231791299</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P9" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q9" s="72"/>
+      <c r="R9" s="72"/>
+      <c r="S9" s="10"/>
+    </row>
+    <row r="10" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -3745,8 +5193,20 @@
         <f>C195</f>
         <v>24.968165588874101</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P10" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q10" s="72">
+        <v>6.64</v>
+      </c>
+      <c r="R10" s="72">
+        <v>6.58</v>
+      </c>
+      <c r="S10" s="10">
+        <v>6.54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -3771,8 +5231,18 @@
         <f>C222</f>
         <v>24.967542195146301</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="P11" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q11" s="72"/>
+      <c r="R11" s="72">
+        <v>6.65</v>
+      </c>
+      <c r="S11" s="10">
+        <v>6.67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -3797,8 +5267,20 @@
         <f>C256</f>
         <v>24.968789013732799</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="P12" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q12" s="72">
+        <v>1.67</v>
+      </c>
+      <c r="R12" s="72">
+        <v>974</v>
+      </c>
+      <c r="S12" s="10">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -3808,8 +5290,20 @@
       <c r="C13" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P13" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q13" s="72">
+        <v>687</v>
+      </c>
+      <c r="R13" s="72">
+        <v>442</v>
+      </c>
+      <c r="S13" s="10">
+        <v>94.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -3826,8 +5320,18 @@
       <c r="M14" s="16" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P14" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q14" s="72"/>
+      <c r="R14" s="72">
+        <v>1.05</v>
+      </c>
+      <c r="S14" s="10">
+        <v>1.84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
@@ -3845,11 +5349,18 @@
         <v>515.10566666666671</v>
       </c>
       <c r="M15" s="10"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-    </row>
-    <row r="16" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P15" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q15" s="73"/>
+      <c r="R15" s="73">
+        <v>568</v>
+      </c>
+      <c r="S15" s="21">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
@@ -6668,9 +8179,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:M2"/>
+    <mergeCell ref="Q2:S2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -15824,8 +17336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FBFCAC3-55BC-944C-B7B3-C5C9963935EC}">
   <dimension ref="C6:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="Q59" sqref="Q59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
enlarge the font of graphs
</commit_message>
<xml_diff>
--- a/LOG8430E_redis_results.xlsx
+++ b/LOG8430E_redis_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thierry/Desktop/LOG8430E_TP3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECDB9684-9464-AF40-897B-5F018EBF203B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529623B3-4373-C94D-95DF-B8C56028BBCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="500" windowWidth="36920" windowHeight="21100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -898,7 +898,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1065,6 +1065,23 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1209,7 +1226,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx2"/>
                     </a:solidFill>
@@ -1269,7 +1286,7 @@
             <c:numRef>
               <c:f>'tps-25'!$L$15:$L$17</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>515.10566666666671</c:v>
@@ -1328,7 +1345,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx2"/>
                     </a:solidFill>
@@ -1388,7 +1405,7 @@
             <c:numRef>
               <c:f>'tps-25'!$M$15:$M$17</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="1">
                   <c:v>1040.9225054652568</c:v>
@@ -1447,7 +1464,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
@@ -1494,7 +1511,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -1504,7 +1521,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US">
+                  <a:rPr lang="en-US" sz="1200">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -1512,7 +1529,7 @@
                   <a:t>Average</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0">
+                  <a:rPr lang="en-US" sz="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -1535,7 +1552,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -1548,7 +1565,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1564,7 +1581,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
@@ -1603,7 +1620,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -2061,7 +2078,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx2"/>
                     </a:solidFill>
@@ -2071,7 +2088,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US">
+                  <a:rPr lang="en-US" sz="1200">
                     <a:solidFill>
                       <a:schemeClr val="tx2"/>
                     </a:solidFill>
@@ -2079,7 +2096,7 @@
                   <a:t>Average</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0">
+                  <a:rPr lang="en-US" sz="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx2"/>
                     </a:solidFill>
@@ -2102,7 +2119,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx2"/>
                   </a:solidFill>
@@ -2137,7 +2154,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx2"/>
                 </a:solidFill>
@@ -2183,7 +2200,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -2193,7 +2210,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US">
+                  <a:rPr lang="en-US" sz="1200">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -2201,7 +2218,7 @@
                   <a:t>Latency</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0">
+                  <a:rPr lang="en-US" sz="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -2224,7 +2241,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -2259,7 +2276,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx2"/>
                 </a:solidFill>
@@ -2310,7 +2327,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -2669,7 +2686,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -2679,7 +2696,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US">
+                  <a:rPr lang="en-US" sz="1200">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -2687,7 +2704,7 @@
                   <a:t>Average</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0">
+                  <a:rPr lang="en-US" sz="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -2710,7 +2727,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -2745,7 +2762,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
@@ -2790,7 +2807,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -2800,7 +2817,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US">
+                  <a:rPr lang="en-US" sz="1200">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -2808,7 +2825,7 @@
                   <a:t>Latency</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0">
+                  <a:rPr lang="en-US" sz="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -2831,7 +2848,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -2866,7 +2883,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
@@ -2913,7 +2930,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -4630,15 +4647,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1016000</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:colOff>1295400</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4947,14 +4964,16 @@
   <dimension ref="A1:S285"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+      <selection activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="9" max="9" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="14" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5397,11 +5416,11 @@
       <c r="K15" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="L15" s="9">
+      <c r="L15" s="82">
         <f>AVERAGE(L4,L7,L10)</f>
         <v>515.10566666666671</v>
       </c>
-      <c r="M15" s="10"/>
+      <c r="M15" s="83"/>
       <c r="P15" s="70" t="s">
         <v>171</v>
       </c>
@@ -5426,11 +5445,11 @@
       <c r="K16" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="L16" s="9">
+      <c r="L16" s="82">
         <f>AVERAGE(L5,L8,L11)</f>
         <v>666.00411489645933</v>
       </c>
-      <c r="M16" s="11">
+      <c r="M16" s="84">
         <f>AVERAGE(M5,M8,M11)</f>
         <v>1040.9225054652568</v>
       </c>
@@ -5450,11 +5469,11 @@
       <c r="K17" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="L17" s="13">
+      <c r="L17" s="85">
         <f>AVERAGE(L6,L9,L12)</f>
         <v>670.74682096041306</v>
       </c>
-      <c r="M17" s="14">
+      <c r="M17" s="86">
         <f>AVERAGE(M6,M9,M12)</f>
         <v>796.91455621109969</v>
       </c>
@@ -14562,7 +14581,7 @@
   <dimension ref="A1:S72"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M51" sqref="M51"/>
+      <selection activeCell="N44" sqref="N44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14581,7 +14600,7 @@
     <col min="13" max="13" width="8.1640625" style="26" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.6640625" style="26" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.33203125" style="26" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.83203125" style="26" customWidth="1"/>
+    <col min="16" max="16" width="15.1640625" style="26" customWidth="1"/>
     <col min="17" max="17" width="13.6640625" style="26" bestFit="1" customWidth="1"/>
     <col min="18" max="16384" width="10.83203125" style="26"/>
   </cols>
@@ -16360,15 +16379,15 @@
         <f>AVERAGE(N6,N10,N14,N18,N22,N26,N30,N34)</f>
         <v>11.14</v>
       </c>
-      <c r="O38" s="34">
+      <c r="O38" s="78">
         <f>AVERAGE(O6,O10,O14,O18,O22,O26,O30,O34)</f>
         <v>0.4603271484375</v>
       </c>
-      <c r="P38" s="34">
+      <c r="P38" s="78">
         <f>AVERAGE(P6,P10,P14,P18,P22,P26,P30,P34) * 1.048576</f>
         <v>6.5541242879999997</v>
       </c>
-      <c r="Q38" s="31">
+      <c r="Q38" s="80">
         <f xml:space="preserve"> 15.55 * 1.073741824</f>
         <v>16.6966853632</v>
       </c>
@@ -16412,15 +16431,15 @@
         <f>AVERAGE(N5,N9,N13,N17,N21,N25,N29,N33)</f>
         <v>11.14</v>
       </c>
-      <c r="O39" s="34">
+      <c r="O39" s="78">
         <f>AVERAGE(O5,O9,O13,O17,O21,O25,O29,O33)</f>
         <v>0.44970703125</v>
       </c>
-      <c r="P39" s="34">
+      <c r="P39" s="78">
         <f>AVERAGE(P5,P9,P13,P17,P21,P25,P29,P33) * 1.048576</f>
         <v>6.5386577919999995</v>
       </c>
-      <c r="Q39" s="31">
+      <c r="Q39" s="80">
         <f xml:space="preserve"> 15.55 * 1.073741824</f>
         <v>16.6966853632</v>
       </c>
@@ -16464,15 +16483,15 @@
         <f>AVERAGE(N4,N8,N12,N16,N20,N24,N28,N32)</f>
         <v>11.14</v>
       </c>
-      <c r="O40" s="34">
+      <c r="O40" s="78">
         <f>AVERAGE(O4,O8,O12,O16,O20,O24,O28,O32)</f>
         <v>0.468994140625</v>
       </c>
-      <c r="P40" s="34">
+      <c r="P40" s="78">
         <f>AVERAGE(P4,P8,P12,P16,P20,P24,P28,P32) * 1.048576</f>
         <v>6.5488814080000006</v>
       </c>
-      <c r="Q40" s="31">
+      <c r="Q40" s="80">
         <f xml:space="preserve"> 15.55 * 1.073741824</f>
         <v>16.6966853632</v>
       </c>
@@ -16516,15 +16535,15 @@
         <f>AVERAGE(N7,N11,N15,N19,N23,N27,N31,N35)</f>
         <v>13.91</v>
       </c>
-      <c r="O41" s="36">
+      <c r="O41" s="79">
         <f>AVERAGE(O7,O11,O15,O19,O23,O27,O31,O35)</f>
         <v>35.5625</v>
       </c>
-      <c r="P41" s="36">
+      <c r="P41" s="79">
         <f>AVERAGE(P7,P11,P15,P19,P23,P27,P31,P35) * 1.048576</f>
         <v>6.3390351360000006</v>
       </c>
-      <c r="Q41" s="32">
+      <c r="Q41" s="81">
         <f xml:space="preserve"> 15.55 * 1.073741824</f>
         <v>16.6966853632</v>
       </c>
@@ -17390,7 +17409,7 @@
   <dimension ref="C6:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="Q59" sqref="Q59"/>
+      <selection activeCell="K59" sqref="K59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
new hyperledger fabric results
</commit_message>
<xml_diff>
--- a/LOG8430E_redis_results.xlsx
+++ b/LOG8430E_redis_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thierry/Desktop/LOG8430E_TP3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5BAF993-757B-6446-9070-225DD7097155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0F9E65-7B68-6C40-827C-C0A8CC995163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="500" windowWidth="36920" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1903,6 +1903,581 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Average Latencies of Hyperleger Fagric Obtained With Caliper With a Throughput of 25 (ops/s)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'tps-25'!$R$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>READ</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'tps-25'!$Q$19:$Q$21</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Workload 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Workload 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Workload 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'tps-25'!$R$19:$R$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4FDC-0646-9556-3CCDF4535BD2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'tps-25'!$S$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WRITES</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'tps-25'!$Q$19:$Q$21</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Workload 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Workload 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Workload 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'tps-25'!$S$20:$S$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.84</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4FDC-0646-9556-3CCDF4535BD2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="341139216"/>
+        <c:axId val="341141216"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="341139216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="341141216"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="341141216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Average </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Latency</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> (us)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="341139216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
               <a:rPr lang="en-US">
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
@@ -2586,7 +3161,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3309,6 +3884,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3813,6 +4428,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4328,7 +5446,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4882,6 +6000,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79400573-2E20-CCA2-5B7C-78CC1E267428}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5166,7 +6320,7 @@
   <dimension ref="A1:Y285"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+      <selection activeCell="V26" sqref="V26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
created diagrams of comparison
</commit_message>
<xml_diff>
--- a/LOG8430E_redis_results.xlsx
+++ b/LOG8430E_redis_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thierry/Desktop/LOG8430E_TP3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0F9E65-7B68-6C40-827C-C0A8CC995163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCE10B4-E712-A14A-A325-AE2C586AD0BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="500" windowWidth="36920" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2209" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2225" uniqueCount="186">
   <si>
     <t>##################################################################################</t>
   </si>
@@ -604,11 +604,23 @@
   <si>
     <t>write Maximum (s)</t>
   </si>
+  <si>
+    <t>YCSB results normalised</t>
+  </si>
+  <si>
+    <t>Caliper results noramlised</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="4">
+    <numFmt numFmtId="165" formatCode="0.000000000"/>
+    <numFmt numFmtId="166" formatCode="0.00000000"/>
+    <numFmt numFmtId="167" formatCode="0.0000000"/>
+    <numFmt numFmtId="168" formatCode="0.000000"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -677,7 +689,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -956,12 +968,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1186,6 +1209,45 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2025,6 +2087,57 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="plus"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'tps-25'!$T$19:$T$21</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.1525</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.02</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.02</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'tps-25'!$T$19:$T$21</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.1525</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.02</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.02</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>'tps-25'!$Q$19:$Q$21</c:f>
@@ -2145,6 +2258,51 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'tps-25'!$U$19:$U$21</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="1">
+                    <c:v>1.5000000000000001E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.5000000000000001E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'tps-25'!$U$19:$U$21</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="1">
+                    <c:v>1.5000000000000001E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.5000000000000001E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>'tps-25'!$Q$19:$Q$21</c:f>
@@ -2164,14 +2322,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'tps-25'!$S$20:$S$21</c:f>
+              <c:f>'tps-25'!$S$19:$S$21</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
+                <c:ptCount val="3"/>
+                <c:pt idx="1">
                   <c:v>0.48</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.84</c:v>
                 </c:pt>
               </c:numCache>
@@ -2304,7 +2462,7 @@
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t> (us)</a:t>
+                  <a:t> (s)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2448,6 +2606,1359 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Comparison between Redis and Hyperledger</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> Reading Latency with a Throughput of 25 (ops/s)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Redis READ</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'tps-25'!$T$27:$T$29</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.1525</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.02</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.02</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'tps-25'!$T$27:$T$29</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.1525</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.02</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.02</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'tps-25'!$K$27:$K$29</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Workload 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Workload 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Workload 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'tps-25'!$L$27:$L$29</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5.1510566666666677E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.6600411489645939E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.7074682096041307E-7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9CD7-8B44-BA25-2A4C2B2C7302}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Hyperledger READ</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'tps-25'!$N$27:$N$29</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>3.5756037494852968E-8</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.2406759739445162E-8</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>6.3996684934322464E-8</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'tps-25'!$N$27:$N$29</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>3.5756037494852968E-8</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.2406759739445162E-8</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>6.3996684934322464E-8</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'tps-25'!$K$27:$K$29</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Workload 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Workload 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Workload 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'tps-25'!$R$27:$R$29</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9CD7-8B44-BA25-2A4C2B2C7302}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="342387552"/>
+        <c:axId val="342389280"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="342387552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="high"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="342389280"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="342389280"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Average </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Latency</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0000000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="342387552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Comparison between Redis and Hyperledger</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> Writing Latency with a Throughput of 25 (ops/s)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Redis Write</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'tps-25'!$U$28:$U$29</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>1.5000000000000001E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.5000000000000001E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'tps-25'!$U$28:$U$29</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>1.5000000000000001E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.5000000000000001E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'tps-25'!$K$27:$K$29</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Workload 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Workload 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Workload 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'tps-25'!$M$28:$M$29</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1.0409225054652568E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.9691455621109979E-7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7E3A-6C4F-A05C-9DD64311FF93}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Hyperledger WRITE</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'tps-25'!$O$28:$O$29</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>3.8117252450149768E-8</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.4929229944012967E-8</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'tps-25'!$O$28:$O$29</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>3.8117252450149768E-8</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.4929229944012967E-8</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'tps-25'!$K$27:$K$29</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Workload 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Workload 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Workload 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'tps-25'!$S$28:$S$29</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.84</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7E3A-6C4F-A05C-9DD64311FF93}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="342387552"/>
+        <c:axId val="342389280"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="342387552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="high"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="342389280"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="342389280"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Average </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Latency</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="342387552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3161,7 +4672,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3885,6 +5396,86 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4931,6 +6522,1012 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5446,7 +8043,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5967,15 +8564,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1295400</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:colOff>1306945</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>131618</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>800100</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>811645</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>157018</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6003,15 +8600,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>430645</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>68118</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>177800</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:colOff>443345</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>118918</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6031,6 +8628,80 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1264227</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>94672</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>761999</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>23091</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5002D9A-2E25-1719-2180-32A73FF4C2AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>230909</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>34636</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>190499</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>159328</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB703387-F84C-C54D-8D5C-75C344BE6C95}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6319,8 +8990,8 @@
   </sheetPr>
   <dimension ref="A1:Y285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="V26" sqref="V26"/>
+    <sheetView tabSelected="1" topLeftCell="I31" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="X66" sqref="X66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6977,7 +9648,7 @@
         <v>0.02</v>
       </c>
       <c r="S19" s="85"/>
-      <c r="T19" s="90">
+      <c r="T19" s="84">
         <f>(W5-W4)/4</f>
         <v>0.1525</v>
       </c>
@@ -7079,7 +9750,7 @@
         <v>25.419999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -7090,7 +9761,7 @@
         <v>1340</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -7100,6 +9771,20 @@
       <c r="C25" s="1">
         <v>1340</v>
       </c>
+      <c r="K25" s="102" t="s">
+        <v>184</v>
+      </c>
+      <c r="L25" s="100"/>
+      <c r="M25" s="100"/>
+      <c r="N25" s="100"/>
+      <c r="O25" s="101"/>
+      <c r="Q25" s="102" t="s">
+        <v>185</v>
+      </c>
+      <c r="R25" s="100"/>
+      <c r="S25" s="100"/>
+      <c r="T25" s="100"/>
+      <c r="U25" s="101"/>
     </row>
     <row r="26" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
@@ -7111,6 +9796,32 @@
       <c r="C26" s="1">
         <v>1340</v>
       </c>
+      <c r="K26" s="5"/>
+      <c r="L26" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="M26" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="N26" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="O26" s="89" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="S26" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="T26" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="U26" s="89" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="27" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
@@ -7122,10 +9833,104 @@
       <c r="C27" s="1">
         <v>1340</v>
       </c>
-    </row>
-    <row r="29" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K27" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="L27" s="103">
+        <f>L16*10^(-9)</f>
+        <v>5.1510566666666677E-7</v>
+      </c>
+      <c r="M27" s="105"/>
+      <c r="N27" s="104">
+        <f>N16*10^(-9)</f>
+        <v>3.5756037494852968E-8</v>
+      </c>
+      <c r="O27" s="106"/>
+      <c r="Q27" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="R27" s="84">
+        <v>0.02</v>
+      </c>
+      <c r="S27" s="85"/>
+      <c r="T27" s="84">
+        <v>0.1525</v>
+      </c>
+      <c r="U27" s="54"/>
+    </row>
+    <row r="28" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K28" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="L28" s="103">
+        <f t="shared" ref="L28:M29" si="0">L17*10^(-9)</f>
+        <v>6.6600411489645939E-7</v>
+      </c>
+      <c r="M28" s="109">
+        <f t="shared" si="0"/>
+        <v>1.0409225054652568E-6</v>
+      </c>
+      <c r="N28" s="104">
+        <f t="shared" ref="N28" si="1">N17*10^(-9)</f>
+        <v>1.2406759739445162E-8</v>
+      </c>
+      <c r="O28" s="111">
+        <f>O17*10^(-9)</f>
+        <v>3.8117252450149768E-8</v>
+      </c>
+      <c r="Q28" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="R28" s="84">
+        <v>0.01</v>
+      </c>
+      <c r="S28" s="86">
+        <v>0.48</v>
+      </c>
+      <c r="T28" s="90">
+        <v>0.02</v>
+      </c>
+      <c r="U28" s="92">
+        <v>1.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="K29" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="L29" s="108">
+        <f t="shared" si="0"/>
+        <v>6.7074682096041307E-7</v>
+      </c>
+      <c r="M29" s="110">
+        <f t="shared" si="0"/>
+        <v>7.9691455621109979E-7</v>
+      </c>
+      <c r="N29" s="107">
+        <f t="shared" ref="N29:O29" si="2">N18*10^(-9)</f>
+        <v>6.3996684934322464E-8</v>
+      </c>
+      <c r="O29" s="112">
+        <f>O18*10^(-9)</f>
+        <v>1.4929229944012967E-8</v>
+      </c>
+      <c r="Q29" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="R29" s="87">
+        <v>0.01</v>
+      </c>
+      <c r="S29" s="88">
+        <v>0.84</v>
+      </c>
+      <c r="T29" s="91">
+        <v>0.02</v>
+      </c>
+      <c r="U29" s="93">
+        <v>1.5000000000000001E-2</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -9778,8 +12583,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
     <mergeCell ref="W6:W7"/>
+    <mergeCell ref="Q25:U25"/>
+    <mergeCell ref="K25:O25"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="R2:T2"/>

</xml_diff>